<commit_message>
adjust comments and round 2
</commit_message>
<xml_diff>
--- a/fine_granularity/results_table/rq3.xlsx
+++ b/fine_granularity/results_table/rq3.xlsx
@@ -602,31 +602,31 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>0.2361219702892885</v>
+        <v>0.24</v>
       </c>
       <c r="C4">
-        <v>0.6138211382113821</v>
+        <v>0.61</v>
       </c>
       <c r="D4">
-        <v>0.3410502540937323</v>
+        <v>0.34</v>
       </c>
       <c r="E4">
-        <v>0.4146341463414634</v>
+        <v>0.41</v>
       </c>
       <c r="F4">
-        <v>0.06390977443609019</v>
+        <v>0.06</v>
       </c>
       <c r="G4">
-        <v>0.1107491856677524</v>
+        <v>0.11</v>
       </c>
       <c r="H4">
-        <v>0.6666666666666666</v>
+        <v>0.67</v>
       </c>
       <c r="I4">
-        <v>0.1126760563380281</v>
+        <v>0.11</v>
       </c>
       <c r="J4">
-        <v>0.1927710843373494</v>
+        <v>0.19</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -638,31 +638,31 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.3333333333333333</v>
+        <v>0.33</v>
       </c>
       <c r="O4">
-        <v>0.0357142857142857</v>
+        <v>0.04</v>
       </c>
       <c r="P4">
-        <v>0.06451612903225799</v>
+        <v>0.06</v>
       </c>
       <c r="Q4">
         <v>0.4</v>
       </c>
       <c r="R4">
-        <v>0.0869565217391304</v>
+        <v>0.09</v>
       </c>
       <c r="S4">
-        <v>0.1428571428571428</v>
+        <v>0.14</v>
       </c>
       <c r="T4">
         <v>1</v>
       </c>
       <c r="U4">
-        <v>0.0114942528735632</v>
+        <v>0.01</v>
       </c>
       <c r="V4">
-        <v>0.0227272727272727</v>
+        <v>0.02</v>
       </c>
       <c r="W4">
         <v>0</v>
@@ -674,22 +674,22 @@
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>0.20703125</v>
+        <v>0.21</v>
       </c>
       <c r="AA4">
-        <v>0.3011363636363636</v>
+        <v>0.3</v>
       </c>
       <c r="AB4">
-        <v>0.2453703703703703</v>
+        <v>0.25</v>
       </c>
       <c r="AC4">
-        <v>0.128876404494382</v>
+        <v>0.13</v>
       </c>
       <c r="AD4">
-        <v>-0.1479920124251165</v>
+        <v>-0.15</v>
       </c>
       <c r="AE4">
-        <v>0.004814899191251887</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:31">
@@ -697,31 +697,31 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>0.07612197028928849</v>
+        <v>0.08</v>
       </c>
       <c r="C5">
-        <v>0.4838211382113821</v>
+        <v>0.48</v>
       </c>
       <c r="D5">
-        <v>0.2010502540937323</v>
+        <v>0.2</v>
       </c>
       <c r="E5">
-        <v>0.3346341463414634</v>
+        <v>0.33</v>
       </c>
       <c r="F5">
-        <v>0.02390977443609019</v>
+        <v>0.02</v>
       </c>
       <c r="G5">
-        <v>0.06074918566775239</v>
+        <v>0.06</v>
       </c>
       <c r="H5">
-        <v>0.5266666666666666</v>
+        <v>0.53</v>
       </c>
       <c r="I5">
-        <v>0.0526760563380281</v>
+        <v>0.05</v>
       </c>
       <c r="J5">
-        <v>0.1127710843373494</v>
+        <v>0.11</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -733,31 +733,31 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.3333333333333333</v>
+        <v>0.33</v>
       </c>
       <c r="O5">
-        <v>0.0357142857142857</v>
+        <v>0.04</v>
       </c>
       <c r="P5">
-        <v>0.06451612903225799</v>
+        <v>0.06</v>
       </c>
       <c r="Q5">
         <v>0.15</v>
       </c>
       <c r="R5">
-        <v>-0.0430434782608696</v>
+        <v>-0.04</v>
       </c>
       <c r="S5">
-        <v>-0.02714285714285722</v>
+        <v>-0.03</v>
       </c>
       <c r="T5">
         <v>0.86</v>
       </c>
       <c r="U5">
-        <v>-0.07850574712643679</v>
+        <v>-0.08</v>
       </c>
       <c r="V5">
-        <v>-0.08727272727272731</v>
+        <v>-0.09</v>
       </c>
       <c r="W5">
         <v>-0.08</v>
@@ -769,22 +769,22 @@
         <v>-0.05</v>
       </c>
       <c r="Z5">
-        <v>0.10703125</v>
+        <v>0.11</v>
       </c>
       <c r="AA5">
-        <v>0.2511363636363636</v>
+        <v>0.25</v>
       </c>
       <c r="AB5">
-        <v>0.1853703703703703</v>
+        <v>0.19</v>
       </c>
       <c r="AC5">
-        <v>0.08887640449438194</v>
+        <v>0.09</v>
       </c>
       <c r="AD5">
-        <v>-0.05799201242511653</v>
+        <v>-0.06</v>
       </c>
       <c r="AE5">
-        <v>0.0248148991912519</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="6" spans="1:31">
@@ -792,31 +792,31 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>0.1361219702892885</v>
+        <v>0.14</v>
       </c>
       <c r="C6">
-        <v>0.5338211382113821</v>
+        <v>0.53</v>
       </c>
       <c r="D6">
-        <v>0.2510502540937323</v>
+        <v>0.25</v>
       </c>
       <c r="E6">
-        <v>0.4146341463414634</v>
+        <v>0.41</v>
       </c>
       <c r="F6">
-        <v>0.06390977443609019</v>
+        <v>0.06</v>
       </c>
       <c r="G6">
-        <v>0.1107491856677524</v>
+        <v>0.11</v>
       </c>
       <c r="H6">
-        <v>0.6666666666666666</v>
+        <v>0.67</v>
       </c>
       <c r="I6">
-        <v>0.1126760563380281</v>
+        <v>0.11</v>
       </c>
       <c r="J6">
-        <v>0.1927710843373494</v>
+        <v>0.19</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -828,31 +828,31 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.3333333333333333</v>
+        <v>0.33</v>
       </c>
       <c r="O6">
-        <v>0.0357142857142857</v>
+        <v>0.04</v>
       </c>
       <c r="P6">
-        <v>0.06451612903225799</v>
+        <v>0.06</v>
       </c>
       <c r="Q6">
         <v>0.4</v>
       </c>
       <c r="R6">
-        <v>0.0869565217391304</v>
+        <v>0.09</v>
       </c>
       <c r="S6">
-        <v>0.1428571428571428</v>
+        <v>0.14</v>
       </c>
       <c r="T6">
         <v>1</v>
       </c>
       <c r="U6">
-        <v>0.0114942528735632</v>
+        <v>0.01</v>
       </c>
       <c r="V6">
-        <v>0.0227272727272727</v>
+        <v>0.02</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -864,22 +864,22 @@
         <v>0</v>
       </c>
       <c r="Z6">
-        <v>-0.02296875000000001</v>
+        <v>-0.02</v>
       </c>
       <c r="AA6">
-        <v>0.2811363636363636</v>
+        <v>0.28</v>
       </c>
       <c r="AB6">
-        <v>0.2053703703703703</v>
+        <v>0.21</v>
       </c>
       <c r="AC6">
-        <v>0.118876404494382</v>
+        <v>0.12</v>
       </c>
       <c r="AD6">
-        <v>-0.08799201242511645</v>
+        <v>-0.09</v>
       </c>
       <c r="AE6">
-        <v>0.0248148991912519</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="7" spans="1:31">
@@ -887,31 +887,31 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>0.2361219702892885</v>
+        <v>0.24</v>
       </c>
       <c r="C7">
-        <v>0.6138211382113821</v>
+        <v>0.61</v>
       </c>
       <c r="D7">
-        <v>0.3410502540937323</v>
+        <v>0.34</v>
       </c>
       <c r="E7">
-        <v>0.4146341463414634</v>
+        <v>0.41</v>
       </c>
       <c r="F7">
-        <v>0.06390977443609019</v>
+        <v>0.06</v>
       </c>
       <c r="G7">
-        <v>0.1107491856677524</v>
+        <v>0.11</v>
       </c>
       <c r="H7">
-        <v>0.5666666666666667</v>
+        <v>0.57</v>
       </c>
       <c r="I7">
-        <v>0.1026760563380281</v>
+        <v>0.1</v>
       </c>
       <c r="J7">
-        <v>0.1727710843373494</v>
+        <v>0.17</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -923,31 +923,31 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0.3333333333333333</v>
+        <v>0.33</v>
       </c>
       <c r="O7">
-        <v>0.0357142857142857</v>
+        <v>0.04</v>
       </c>
       <c r="P7">
-        <v>0.06451612903225799</v>
+        <v>0.06</v>
       </c>
       <c r="Q7">
         <v>0.4</v>
       </c>
       <c r="R7">
-        <v>0.0869565217391304</v>
+        <v>0.09</v>
       </c>
       <c r="S7">
-        <v>0.1428571428571428</v>
+        <v>0.14</v>
       </c>
       <c r="T7">
         <v>1</v>
       </c>
       <c r="U7">
-        <v>0.0114942528735632</v>
+        <v>0.01</v>
       </c>
       <c r="V7">
-        <v>0.0227272727272727</v>
+        <v>0.02</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -959,22 +959,22 @@
         <v>0</v>
       </c>
       <c r="Z7">
-        <v>0.16703125</v>
+        <v>0.17</v>
       </c>
       <c r="AA7">
-        <v>0.2811363636363636</v>
+        <v>0.28</v>
       </c>
       <c r="AB7">
-        <v>0.2153703703703703</v>
+        <v>0.22</v>
       </c>
       <c r="AC7">
-        <v>0.128876404494382</v>
+        <v>0.13</v>
       </c>
       <c r="AD7">
-        <v>-0.1379920124251165</v>
+        <v>-0.14</v>
       </c>
       <c r="AE7">
-        <v>0.004814899191251887</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:31">
@@ -982,31 +982,31 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>0.2361219702892885</v>
+        <v>0.24</v>
       </c>
       <c r="C8">
-        <v>0.6138211382113821</v>
+        <v>0.61</v>
       </c>
       <c r="D8">
-        <v>0.3410502540937323</v>
+        <v>0.34</v>
       </c>
       <c r="E8">
-        <v>0.4146341463414634</v>
+        <v>0.41</v>
       </c>
       <c r="F8">
-        <v>0.06390977443609019</v>
+        <v>0.06</v>
       </c>
       <c r="G8">
-        <v>0.1107491856677524</v>
+        <v>0.11</v>
       </c>
       <c r="H8">
-        <v>0.6666666666666666</v>
+        <v>0.67</v>
       </c>
       <c r="I8">
-        <v>0.1126760563380281</v>
+        <v>0.11</v>
       </c>
       <c r="J8">
-        <v>0.1927710843373494</v>
+        <v>0.19</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1018,31 +1018,31 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>0.3333333333333333</v>
+        <v>0.33</v>
       </c>
       <c r="O8">
-        <v>0.0357142857142857</v>
+        <v>0.04</v>
       </c>
       <c r="P8">
-        <v>0.06451612903225799</v>
+        <v>0.06</v>
       </c>
       <c r="Q8">
         <v>0.4</v>
       </c>
       <c r="R8">
-        <v>0.0869565217391304</v>
+        <v>0.09</v>
       </c>
       <c r="S8">
-        <v>0.1428571428571428</v>
+        <v>0.14</v>
       </c>
       <c r="T8">
         <v>1</v>
       </c>
       <c r="U8">
-        <v>0.0114942528735632</v>
+        <v>0.01</v>
       </c>
       <c r="V8">
-        <v>0.0227272727272727</v>
+        <v>0.02</v>
       </c>
       <c r="W8">
         <v>0</v>
@@ -1054,22 +1054,22 @@
         <v>0</v>
       </c>
       <c r="Z8">
-        <v>0.20703125</v>
+        <v>0.21</v>
       </c>
       <c r="AA8">
-        <v>0.3011363636363636</v>
+        <v>0.3</v>
       </c>
       <c r="AB8">
-        <v>0.2453703703703703</v>
+        <v>0.25</v>
       </c>
       <c r="AC8">
-        <v>0.128876404494382</v>
+        <v>0.13</v>
       </c>
       <c r="AD8">
-        <v>-0.1479920124251165</v>
+        <v>-0.15</v>
       </c>
       <c r="AE8">
-        <v>0.004814899191251887</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:31">
@@ -1077,31 +1077,31 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>-0.0138780297107115</v>
+        <v>-0.01</v>
       </c>
       <c r="C9">
-        <v>0.563821138211382</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="D9">
-        <v>0.2610502540937323</v>
+        <v>0.26</v>
       </c>
       <c r="E9">
-        <v>0.2646341463414634</v>
+        <v>0.26</v>
       </c>
       <c r="F9">
-        <v>0.05390977443609019</v>
+        <v>0.05</v>
       </c>
       <c r="G9">
-        <v>0.1007491856677524</v>
+        <v>0.1</v>
       </c>
       <c r="H9">
-        <v>0.5666666666666667</v>
+        <v>0.57</v>
       </c>
       <c r="I9">
-        <v>0.1026760563380281</v>
+        <v>0.1</v>
       </c>
       <c r="J9">
-        <v>0.1727710843373494</v>
+        <v>0.17</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1113,31 +1113,31 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0.3333333333333333</v>
+        <v>0.33</v>
       </c>
       <c r="O9">
-        <v>0.0357142857142857</v>
+        <v>0.04</v>
       </c>
       <c r="P9">
-        <v>0.06451612903225799</v>
+        <v>0.06</v>
       </c>
       <c r="Q9">
         <v>0.4</v>
       </c>
       <c r="R9">
-        <v>0.0869565217391304</v>
+        <v>0.09</v>
       </c>
       <c r="S9">
-        <v>0.1428571428571428</v>
+        <v>0.14</v>
       </c>
       <c r="T9">
         <v>1</v>
       </c>
       <c r="U9">
-        <v>0.0114942528735632</v>
+        <v>0.01</v>
       </c>
       <c r="V9">
-        <v>0.0227272727272727</v>
+        <v>0.02</v>
       </c>
       <c r="W9">
         <v>0</v>
@@ -1149,22 +1149,22 @@
         <v>0</v>
       </c>
       <c r="Z9">
-        <v>0.17703125</v>
+        <v>0.18</v>
       </c>
       <c r="AA9">
-        <v>0.2911363636363636</v>
+        <v>0.29</v>
       </c>
       <c r="AB9">
-        <v>0.2353703703703703</v>
+        <v>0.24</v>
       </c>
       <c r="AC9">
-        <v>0.118876404494382</v>
+        <v>0.12</v>
       </c>
       <c r="AD9">
-        <v>-0.1379920124251165</v>
+        <v>-0.14</v>
       </c>
       <c r="AE9">
-        <v>0.004814899191251887</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:31">
@@ -1172,31 +1172,31 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <v>0.2361219702892885</v>
+        <v>0.24</v>
       </c>
       <c r="C10">
-        <v>0.6138211382113821</v>
+        <v>0.61</v>
       </c>
       <c r="D10">
-        <v>0.3410502540937323</v>
+        <v>0.34</v>
       </c>
       <c r="E10">
-        <v>0.4146341463414634</v>
+        <v>0.41</v>
       </c>
       <c r="F10">
-        <v>0.06390977443609019</v>
+        <v>0.06</v>
       </c>
       <c r="G10">
-        <v>0.1107491856677524</v>
+        <v>0.11</v>
       </c>
       <c r="H10">
-        <v>0.6666666666666666</v>
+        <v>0.67</v>
       </c>
       <c r="I10">
-        <v>0.1126760563380281</v>
+        <v>0.11</v>
       </c>
       <c r="J10">
-        <v>0.1927710843373494</v>
+        <v>0.19</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1208,31 +1208,31 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0.3333333333333333</v>
+        <v>0.33</v>
       </c>
       <c r="O10">
-        <v>0.0357142857142857</v>
+        <v>0.04</v>
       </c>
       <c r="P10">
-        <v>0.06451612903225799</v>
+        <v>0.06</v>
       </c>
       <c r="Q10">
         <v>0.4</v>
       </c>
       <c r="R10">
-        <v>0.0869565217391304</v>
+        <v>0.09</v>
       </c>
       <c r="S10">
-        <v>0.1428571428571428</v>
+        <v>0.14</v>
       </c>
       <c r="T10">
         <v>1</v>
       </c>
       <c r="U10">
-        <v>0.0114942528735632</v>
+        <v>0.01</v>
       </c>
       <c r="V10">
-        <v>0.0227272727272727</v>
+        <v>0.02</v>
       </c>
       <c r="W10">
         <v>0</v>
@@ -1244,22 +1244,22 @@
         <v>0</v>
       </c>
       <c r="Z10">
-        <v>0.20703125</v>
+        <v>0.21</v>
       </c>
       <c r="AA10">
-        <v>0.3011363636363636</v>
+        <v>0.3</v>
       </c>
       <c r="AB10">
-        <v>0.2453703703703703</v>
+        <v>0.25</v>
       </c>
       <c r="AC10">
-        <v>0.128876404494382</v>
+        <v>0.13</v>
       </c>
       <c r="AD10">
-        <v>-0.1479920124251165</v>
+        <v>-0.15</v>
       </c>
       <c r="AE10">
-        <v>0.004814899191251887</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:31">
@@ -1267,31 +1267,31 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>0.2361219702892885</v>
+        <v>0.24</v>
       </c>
       <c r="C11">
-        <v>0.6138211382113821</v>
+        <v>0.61</v>
       </c>
       <c r="D11">
-        <v>0.3410502540937323</v>
+        <v>0.34</v>
       </c>
       <c r="E11">
-        <v>0.4146341463414634</v>
+        <v>0.41</v>
       </c>
       <c r="F11">
-        <v>0.06390977443609019</v>
+        <v>0.06</v>
       </c>
       <c r="G11">
-        <v>0.1107491856677524</v>
+        <v>0.11</v>
       </c>
       <c r="H11">
-        <v>0.6666666666666666</v>
+        <v>0.67</v>
       </c>
       <c r="I11">
-        <v>0.1126760563380281</v>
+        <v>0.11</v>
       </c>
       <c r="J11">
-        <v>0.1927710843373494</v>
+        <v>0.19</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1303,31 +1303,31 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.3333333333333333</v>
+        <v>0.33</v>
       </c>
       <c r="O11">
-        <v>0.0357142857142857</v>
+        <v>0.04</v>
       </c>
       <c r="P11">
-        <v>0.06451612903225799</v>
+        <v>0.06</v>
       </c>
       <c r="Q11">
         <v>0.4</v>
       </c>
       <c r="R11">
-        <v>0.0869565217391304</v>
+        <v>0.09</v>
       </c>
       <c r="S11">
-        <v>0.1428571428571428</v>
+        <v>0.14</v>
       </c>
       <c r="T11">
         <v>1</v>
       </c>
       <c r="U11">
-        <v>0.0114942528735632</v>
+        <v>0.01</v>
       </c>
       <c r="V11">
-        <v>0.0227272727272727</v>
+        <v>0.02</v>
       </c>
       <c r="W11">
         <v>0</v>
@@ -1339,22 +1339,22 @@
         <v>0</v>
       </c>
       <c r="Z11">
-        <v>0.16703125</v>
+        <v>0.17</v>
       </c>
       <c r="AA11">
-        <v>0.2811363636363636</v>
+        <v>0.28</v>
       </c>
       <c r="AB11">
-        <v>0.2253703703703703</v>
+        <v>0.23</v>
       </c>
       <c r="AC11">
-        <v>0.128876404494382</v>
+        <v>0.13</v>
       </c>
       <c r="AD11">
-        <v>-0.1379920124251165</v>
+        <v>-0.14</v>
       </c>
       <c r="AE11">
-        <v>0.004814899191251887</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:31">
@@ -1362,31 +1362,31 @@
         <v>22</v>
       </c>
       <c r="B12">
-        <v>-0.04387802971071153</v>
+        <v>-0.04</v>
       </c>
       <c r="C12">
-        <v>0.2838211382113821</v>
+        <v>0.28</v>
       </c>
       <c r="D12">
-        <v>0.0310502540937323</v>
+        <v>0.03</v>
       </c>
       <c r="E12">
-        <v>0.1846341463414634</v>
+        <v>0.18</v>
       </c>
       <c r="F12">
-        <v>-0.006090225563909812</v>
+        <v>-0.01</v>
       </c>
       <c r="G12">
-        <v>0.0007491856677523945</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>0.1766666666666666</v>
+        <v>0.18</v>
       </c>
       <c r="I12">
-        <v>-0.2373239436619719</v>
+        <v>-0.24</v>
       </c>
       <c r="J12">
-        <v>-0.2072289156626506</v>
+        <v>-0.21</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1398,31 +1398,31 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0.3333333333333333</v>
+        <v>0.33</v>
       </c>
       <c r="O12">
-        <v>0.0357142857142857</v>
+        <v>0.04</v>
       </c>
       <c r="P12">
-        <v>0.06451612903225799</v>
+        <v>0.06</v>
       </c>
       <c r="Q12">
         <v>0.4</v>
       </c>
       <c r="R12">
-        <v>0.0869565217391304</v>
+        <v>0.09</v>
       </c>
       <c r="S12">
-        <v>0.1428571428571428</v>
+        <v>0.14</v>
       </c>
       <c r="T12">
         <v>0.73</v>
       </c>
       <c r="U12">
-        <v>-0.1085057471264368</v>
+        <v>-0.11</v>
       </c>
       <c r="V12">
-        <v>-0.1372727272727273</v>
+        <v>-0.14</v>
       </c>
       <c r="W12">
         <v>0</v>
@@ -1434,22 +1434,22 @@
         <v>0</v>
       </c>
       <c r="Z12">
-        <v>-0.02296875000000001</v>
+        <v>-0.02</v>
       </c>
       <c r="AA12">
-        <v>0.1811363636363636</v>
+        <v>0.18</v>
       </c>
       <c r="AB12">
-        <v>0.0953703703703703</v>
+        <v>0.1</v>
       </c>
       <c r="AC12">
-        <v>0.04887640449438202</v>
+        <v>0.05</v>
       </c>
       <c r="AD12">
-        <v>-0.08799201242511645</v>
+        <v>-0.09</v>
       </c>
       <c r="AE12">
-        <v>-0.02518510080874814</v>
+        <v>-0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>